<commit_message>
Updated ITA_grids model - 2025-09-02 19:34
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA_grids/SuppXLS/scen_tsparameters_ts_annual.xlsx
+++ b/VerveStacks_ITA_grids/SuppXLS/scen_tsparameters_ts_annual.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA_grids\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C37F28B5-6E37-4D39-8C92-C64FCD5DCE9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{77F7A3C4-6771-4C0A-B866-F0589AA62261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="1" activeTab="1" xr2:uid="{693B72C3-6B34-4E45-9416-347F2176C33F}"/>
   </bookViews>
@@ -3726,7 +3726,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B5F16A9-FF5E-4E0D-9195-1A2CD326951C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB824E1B-60E2-46DD-9A5D-D68170613D70}">
   <dimension ref="A9:AM335"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>